<commit_message>
Updated IssuesDatesOrdered+IssuesPer Month to show the data we have
</commit_message>
<xml_diff>
--- a/GhTorrentSQL Data/IssueDatesOrdered+IssuesPerMonth.xlsx
+++ b/GhTorrentSQL Data/IssueDatesOrdered+IssuesPerMonth.xlsx
@@ -17,12 +17,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">IssueDatesOrdered!$A$1:$E$515</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="19">
   <si>
     <t>name</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>December</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -893,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S515"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -974,29 +977,29 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="H2" s="2">
-        <v>0</v>
-      </c>
-      <c r="I2" s="2">
-        <v>0</v>
-      </c>
-      <c r="J2" s="2">
-        <v>0</v>
-      </c>
-      <c r="K2" s="2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2" s="2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
+      <c r="H2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" t="s">
+        <v>18</v>
       </c>
       <c r="P2" s="2">
         <v>4</v>
@@ -1100,28 +1103,28 @@
       <c r="E5">
         <v>4</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <v>11</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="2">
         <v>3</v>
       </c>
       <c r="J5" s="2">
         <v>36</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="2">
         <v>2</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="2">
         <v>4</v>
       </c>
       <c r="M5" s="2">
         <v>57</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="2">
         <v>17</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="2">
         <v>5</v>
       </c>
       <c r="P5" s="2">
@@ -1133,7 +1136,7 @@
       <c r="R5">
         <v>13</v>
       </c>
-      <c r="S5">
+      <c r="S5" s="2">
         <v>8</v>
       </c>
     </row>

</xml_diff>